<commit_message>
Added DCF and WACC initializers.
</commit_message>
<xml_diff>
--- a/src/main/resources/companies/template.xlsx
+++ b/src/main/resources/companies/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Valuation Metrics" sheetId="5" r:id="rId1"/>
@@ -1415,6 +1415,9 @@
     <xf numFmtId="10" fontId="11" fillId="3" borderId="5" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1492,9 +1495,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="4" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="20% - Accent1" xfId="9" builtinId="30"/>
@@ -2115,11 +2115,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="358191240"/>
-        <c:axId val="358191624"/>
+        <c:axId val="133839888"/>
+        <c:axId val="133837536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="358191240"/>
+        <c:axId val="133839888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2161,7 +2161,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358191624"/>
+        <c:crossAx val="133837536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2169,7 +2169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358191624"/>
+        <c:axId val="133837536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2272,7 +2272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358191240"/>
+        <c:crossAx val="133839888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2877,11 +2877,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="359338400"/>
-        <c:axId val="359339184"/>
+        <c:axId val="357086440"/>
+        <c:axId val="357084088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359338400"/>
+        <c:axId val="357086440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2923,7 +2923,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359339184"/>
+        <c:crossAx val="357084088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2931,7 +2931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359339184"/>
+        <c:axId val="357084088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2981,7 +2981,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359338400"/>
+        <c:crossAx val="357086440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3327,11 +3327,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="359339968"/>
-        <c:axId val="359334872"/>
+        <c:axId val="357088400"/>
+        <c:axId val="357089968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="359339968"/>
+        <c:axId val="357088400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3373,7 +3373,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359334872"/>
+        <c:crossAx val="357089968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3381,7 +3381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359334872"/>
+        <c:axId val="357089968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3431,7 +3431,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359339968"/>
+        <c:crossAx val="357088400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3892,8 +3892,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="358612440"/>
-        <c:axId val="358629224"/>
+        <c:axId val="133839104"/>
+        <c:axId val="133838320"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -4031,11 +4031,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="358629992"/>
-        <c:axId val="358629608"/>
+        <c:axId val="356441048"/>
+        <c:axId val="133840280"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="358612440"/>
+        <c:axId val="133839104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4077,7 +4077,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358629224"/>
+        <c:crossAx val="133838320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4085,7 +4085,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358629224"/>
+        <c:axId val="133838320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4135,12 +4135,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358612440"/>
+        <c:crossAx val="133839104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358629608"/>
+        <c:axId val="133840280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4176,12 +4176,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358629992"/>
+        <c:crossAx val="356441048"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="358629992"/>
+        <c:axId val="356441048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4190,7 +4190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="358629608"/>
+        <c:crossAx val="133840280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4689,11 +4689,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="358711920"/>
-        <c:axId val="358712304"/>
+        <c:axId val="356439480"/>
+        <c:axId val="356443792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="358711920"/>
+        <c:axId val="356439480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4735,7 +4735,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358712304"/>
+        <c:crossAx val="356443792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4743,7 +4743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358712304"/>
+        <c:axId val="356443792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4793,7 +4793,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358711920"/>
+        <c:crossAx val="356439480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5255,11 +5255,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="358733056"/>
-        <c:axId val="358851712"/>
+        <c:axId val="356438304"/>
+        <c:axId val="356445360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="358733056"/>
+        <c:axId val="356438304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5301,7 +5301,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358851712"/>
+        <c:crossAx val="356445360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5309,7 +5309,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="358851712"/>
+        <c:axId val="356445360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5359,7 +5359,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358733056"/>
+        <c:crossAx val="356438304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5800,8 +5800,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="358777552"/>
-        <c:axId val="359173888"/>
+        <c:axId val="356439088"/>
+        <c:axId val="356439872"/>
       </c:barChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -5939,11 +5939,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="359171928"/>
-        <c:axId val="359172712"/>
+        <c:axId val="356443008"/>
+        <c:axId val="356440264"/>
       </c:scatterChart>
       <c:catAx>
-        <c:axId val="358777552"/>
+        <c:axId val="356439088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5985,7 +5985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359173888"/>
+        <c:crossAx val="356439872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5993,7 +5993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359173888"/>
+        <c:axId val="356439872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6043,12 +6043,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="358777552"/>
+        <c:crossAx val="356439088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359172712"/>
+        <c:axId val="356440264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6084,12 +6084,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359171928"/>
+        <c:crossAx val="356443008"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359171928"/>
+        <c:axId val="356443008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6098,7 +6098,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="359172712"/>
+        <c:crossAx val="356440264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6519,8 +6519,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="359174672"/>
-        <c:axId val="359171536"/>
+        <c:axId val="356440656"/>
+        <c:axId val="356441440"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="stacked"/>
@@ -6699,11 +6699,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="359174280"/>
-        <c:axId val="359175064"/>
+        <c:axId val="356444184"/>
+        <c:axId val="356441832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359174672"/>
+        <c:axId val="356440656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6745,7 +6745,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359171536"/>
+        <c:crossAx val="356441440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6753,7 +6753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359171536"/>
+        <c:axId val="356441440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6803,12 +6803,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359174672"/>
+        <c:crossAx val="356440656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="359175064"/>
+        <c:axId val="356441832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6844,12 +6844,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359174280"/>
+        <c:crossAx val="356444184"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="359174280"/>
+        <c:axId val="356444184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6886,7 +6886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359175064"/>
+        <c:crossAx val="356441832"/>
         <c:crosses val="max"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7860,11 +7860,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="359336048"/>
-        <c:axId val="359173104"/>
+        <c:axId val="357084480"/>
+        <c:axId val="356442616"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="359173104"/>
+        <c:axId val="356442616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7914,12 +7914,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359336048"/>
+        <c:crossAx val="357084480"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="359336048"/>
+        <c:axId val="357084480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7961,7 +7961,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359173104"/>
+        <c:crossAx val="356442616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8628,11 +8628,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="359337616"/>
-        <c:axId val="359336832"/>
+        <c:axId val="357087224"/>
+        <c:axId val="357083304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="359337616"/>
+        <c:axId val="357087224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8693,7 +8693,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359336832"/>
+        <c:crossAx val="357083304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8701,7 +8701,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359336832"/>
+        <c:axId val="357083304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8762,7 +8762,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359337616"/>
+        <c:crossAx val="357087224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9112,11 +9112,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="359337224"/>
-        <c:axId val="359335656"/>
+        <c:axId val="357089576"/>
+        <c:axId val="357086048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="359337224"/>
+        <c:axId val="357089576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9158,7 +9158,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359335656"/>
+        <c:crossAx val="357086048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9166,7 +9166,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="359335656"/>
+        <c:axId val="357086048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9216,7 +9216,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="359337224"/>
+        <c:crossAx val="357089576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16430,7 +16430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
@@ -16446,74 +16446,74 @@
   <sheetData>
     <row r="2" spans="2:22" ht="15" thickBot="1"/>
     <row r="3" spans="2:22">
-      <c r="B3" s="138" t="s">
+      <c r="B3" s="139" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="139"/>
-      <c r="D3" s="139"/>
-      <c r="E3" s="139"/>
-      <c r="F3" s="139"/>
-      <c r="G3" s="139"/>
-      <c r="H3" s="139"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="139"/>
-      <c r="K3" s="139"/>
-      <c r="L3" s="139"/>
-      <c r="M3" s="139"/>
-      <c r="N3" s="139"/>
-      <c r="O3" s="139"/>
-      <c r="P3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="140"/>
+      <c r="N3" s="140"/>
+      <c r="O3" s="140"/>
+      <c r="P3" s="141"/>
     </row>
     <row r="4" spans="2:22">
-      <c r="B4" s="141"/>
-      <c r="C4" s="142"/>
-      <c r="D4" s="142"/>
-      <c r="E4" s="142"/>
-      <c r="F4" s="142"/>
-      <c r="G4" s="142"/>
-      <c r="H4" s="142"/>
-      <c r="I4" s="142"/>
-      <c r="J4" s="142"/>
-      <c r="K4" s="142"/>
-      <c r="L4" s="142"/>
-      <c r="M4" s="142"/>
-      <c r="N4" s="142"/>
-      <c r="O4" s="142"/>
-      <c r="P4" s="143"/>
+      <c r="B4" s="142"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="143"/>
+      <c r="L4" s="143"/>
+      <c r="M4" s="143"/>
+      <c r="N4" s="143"/>
+      <c r="O4" s="143"/>
+      <c r="P4" s="144"/>
     </row>
     <row r="5" spans="2:22">
-      <c r="B5" s="141"/>
-      <c r="C5" s="142"/>
-      <c r="D5" s="142"/>
-      <c r="E5" s="142"/>
-      <c r="F5" s="142"/>
-      <c r="G5" s="142"/>
-      <c r="H5" s="142"/>
-      <c r="I5" s="142"/>
-      <c r="J5" s="142"/>
-      <c r="K5" s="142"/>
-      <c r="L5" s="142"/>
-      <c r="M5" s="142"/>
-      <c r="N5" s="142"/>
-      <c r="O5" s="142"/>
-      <c r="P5" s="143"/>
+      <c r="B5" s="142"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
+      <c r="H5" s="143"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="143"/>
+      <c r="N5" s="143"/>
+      <c r="O5" s="143"/>
+      <c r="P5" s="144"/>
     </row>
     <row r="6" spans="2:22" ht="15" thickBot="1">
-      <c r="B6" s="144"/>
-      <c r="C6" s="145"/>
-      <c r="D6" s="145"/>
-      <c r="E6" s="145"/>
-      <c r="F6" s="145"/>
-      <c r="G6" s="145"/>
-      <c r="H6" s="145"/>
-      <c r="I6" s="145"/>
-      <c r="J6" s="145"/>
-      <c r="K6" s="145"/>
-      <c r="L6" s="145"/>
-      <c r="M6" s="145"/>
-      <c r="N6" s="145"/>
-      <c r="O6" s="145"/>
-      <c r="P6" s="146"/>
+      <c r="B6" s="145"/>
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="146"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="146"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="146"/>
+      <c r="L6" s="146"/>
+      <c r="M6" s="146"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="146"/>
+      <c r="P6" s="147"/>
     </row>
     <row r="8" spans="2:22" ht="13.5" customHeight="1"/>
     <row r="10" spans="2:22" ht="17.5" thickBot="1">
@@ -16562,7 +16562,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" ht="19" thickTop="1">
-      <c r="B11" s="147" t="s">
+      <c r="B11" s="148" t="s">
         <v>89</v>
       </c>
       <c r="C11" s="35"/>
@@ -16590,7 +16590,7 @@
       </c>
     </row>
     <row r="12" spans="2:22" ht="18.5">
-      <c r="B12" s="148"/>
+      <c r="B12" s="149"/>
       <c r="C12" s="35" t="s">
         <v>155</v>
       </c>
@@ -16646,7 +16646,7 @@
       </c>
     </row>
     <row r="13" spans="2:22">
-      <c r="B13" s="148"/>
+      <c r="B13" s="149"/>
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
       <c r="E13" s="45"/>
@@ -16663,7 +16663,7 @@
       <c r="P13" s="128"/>
     </row>
     <row r="14" spans="2:22" ht="18.5">
-      <c r="B14" s="149"/>
+      <c r="B14" s="150"/>
       <c r="C14" s="35" t="s">
         <v>156</v>
       </c>
@@ -16722,7 +16722,7 @@
       <c r="T14" s="44"/>
     </row>
     <row r="15" spans="2:22">
-      <c r="B15" s="149"/>
+      <c r="B15" s="150"/>
       <c r="C15" s="35"/>
       <c r="D15" s="35"/>
       <c r="E15" s="45"/>
@@ -16742,7 +16742,7 @@
       <c r="T15" s="44"/>
     </row>
     <row r="16" spans="2:22" ht="18.5">
-      <c r="B16" s="149"/>
+      <c r="B16" s="150"/>
       <c r="C16" s="35" t="s">
         <v>157</v>
       </c>
@@ -16802,7 +16802,7 @@
       <c r="T16" s="44"/>
     </row>
     <row r="17" spans="2:20">
-      <c r="B17" s="150" t="s">
+      <c r="B17" s="151" t="s">
         <v>65</v>
       </c>
       <c r="C17" s="36"/>
@@ -16825,7 +16825,7 @@
       <c r="T17" s="44"/>
     </row>
     <row r="18" spans="2:20" ht="18.5">
-      <c r="B18" s="151"/>
+      <c r="B18" s="152"/>
       <c r="C18" s="36" t="s">
         <v>158</v>
       </c>
@@ -16885,7 +16885,7 @@
       <c r="T18" s="44"/>
     </row>
     <row r="19" spans="2:20">
-      <c r="B19" s="151"/>
+      <c r="B19" s="152"/>
       <c r="C19" s="36"/>
       <c r="D19" s="36"/>
       <c r="E19" s="48"/>
@@ -16906,7 +16906,7 @@
       <c r="T19" s="44"/>
     </row>
     <row r="20" spans="2:20" ht="18.5">
-      <c r="B20" s="151"/>
+      <c r="B20" s="152"/>
       <c r="C20" s="36" t="s">
         <v>159</v>
       </c>
@@ -16966,7 +16966,7 @@
       <c r="T20" s="44"/>
     </row>
     <row r="21" spans="2:20">
-      <c r="B21" s="156" t="s">
+      <c r="B21" s="157" t="s">
         <v>96</v>
       </c>
       <c r="C21" s="35"/>
@@ -16989,7 +16989,7 @@
       <c r="T21" s="44"/>
     </row>
     <row r="22" spans="2:20" ht="18.5">
-      <c r="B22" s="156"/>
+      <c r="B22" s="157"/>
       <c r="C22" s="35" t="s">
         <v>148</v>
       </c>
@@ -17046,7 +17046,7 @@
       <c r="T22" s="44"/>
     </row>
     <row r="23" spans="2:20">
-      <c r="B23" s="154" t="s">
+      <c r="B23" s="155" t="s">
         <v>95</v>
       </c>
       <c r="C23" s="36"/>
@@ -17069,7 +17069,7 @@
       <c r="T23" s="44"/>
     </row>
     <row r="24" spans="2:20" ht="18.5">
-      <c r="B24" s="155"/>
+      <c r="B24" s="156"/>
       <c r="C24" s="36" t="s">
         <v>98</v>
       </c>
@@ -17129,7 +17129,7 @@
       <c r="T24" s="44"/>
     </row>
     <row r="25" spans="2:20">
-      <c r="B25" s="155"/>
+      <c r="B25" s="156"/>
       <c r="C25" s="36"/>
       <c r="D25" s="36"/>
       <c r="E25" s="51"/>
@@ -17150,7 +17150,7 @@
       <c r="T25" s="44"/>
     </row>
     <row r="26" spans="2:20" ht="18.5">
-      <c r="B26" s="155"/>
+      <c r="B26" s="156"/>
       <c r="C26" s="36" t="s">
         <v>106</v>
       </c>
@@ -17210,7 +17210,7 @@
       <c r="T26" s="44"/>
     </row>
     <row r="27" spans="2:20">
-      <c r="B27" s="155"/>
+      <c r="B27" s="156"/>
       <c r="C27" s="36"/>
       <c r="D27" s="36"/>
       <c r="E27" s="51"/>
@@ -17227,7 +17227,7 @@
       <c r="P27" s="38"/>
     </row>
     <row r="28" spans="2:20" ht="18.5">
-      <c r="B28" s="155"/>
+      <c r="B28" s="156"/>
       <c r="C28" s="36" t="s">
         <v>73</v>
       </c>
@@ -17237,7 +17237,7 @@
       <c r="E28" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="F28" s="164">
+      <c r="F28" s="137">
         <f>Financials!$C$92</f>
         <v>0</v>
       </c>
@@ -17253,7 +17253,7 @@
       <c r="P28" s="38"/>
     </row>
     <row r="29" spans="2:20">
-      <c r="B29" s="152" t="s">
+      <c r="B29" s="153" t="s">
         <v>94</v>
       </c>
       <c r="C29" s="34"/>
@@ -17262,7 +17262,7 @@
       <c r="F29" s="34"/>
     </row>
     <row r="30" spans="2:20" ht="18.5">
-      <c r="B30" s="152"/>
+      <c r="B30" s="153"/>
       <c r="C30" s="35" t="s">
         <v>78</v>
       </c>
@@ -17278,7 +17278,7 @@
       </c>
     </row>
     <row r="31" spans="2:20" ht="18.5">
-      <c r="B31" s="153"/>
+      <c r="B31" s="154"/>
       <c r="C31" s="35" t="s">
         <v>82</v>
       </c>
@@ -17294,14 +17294,14 @@
       </c>
     </row>
     <row r="32" spans="2:20">
-      <c r="B32" s="153"/>
+      <c r="B32" s="154"/>
       <c r="C32" s="35"/>
       <c r="D32" s="35"/>
       <c r="E32" s="50"/>
       <c r="F32" s="52"/>
     </row>
     <row r="33" spans="2:17" ht="18.5">
-      <c r="B33" s="153"/>
+      <c r="B33" s="154"/>
       <c r="C33" s="35" t="s">
         <v>92</v>
       </c>
@@ -17317,7 +17317,7 @@
       </c>
     </row>
     <row r="34" spans="2:17" ht="18.5">
-      <c r="B34" s="153"/>
+      <c r="B34" s="154"/>
       <c r="C34" s="35" t="s">
         <v>93</v>
       </c>
@@ -17333,7 +17333,7 @@
       </c>
     </row>
     <row r="35" spans="2:17">
-      <c r="B35" s="153"/>
+      <c r="B35" s="154"/>
       <c r="C35" s="35"/>
       <c r="D35" s="35"/>
       <c r="E35" s="50"/>
@@ -17341,7 +17341,7 @@
       <c r="Q35" s="37"/>
     </row>
     <row r="36" spans="2:17" ht="18.5">
-      <c r="B36" s="153"/>
+      <c r="B36" s="154"/>
       <c r="C36" s="35" t="s">
         <v>80</v>
       </c>
@@ -17357,7 +17357,7 @@
       </c>
     </row>
     <row r="37" spans="2:17" ht="18.5">
-      <c r="B37" s="153"/>
+      <c r="B37" s="154"/>
       <c r="C37" s="35" t="s">
         <v>83</v>
       </c>
@@ -17373,14 +17373,14 @@
       </c>
     </row>
     <row r="38" spans="2:17">
-      <c r="B38" s="153"/>
+      <c r="B38" s="154"/>
       <c r="C38" s="35"/>
       <c r="D38" s="35"/>
       <c r="E38" s="50"/>
       <c r="F38" s="53"/>
     </row>
     <row r="39" spans="2:17" ht="18.5">
-      <c r="B39" s="153"/>
+      <c r="B39" s="154"/>
       <c r="C39" s="35" t="s">
         <v>81</v>
       </c>
@@ -17396,7 +17396,7 @@
       </c>
     </row>
     <row r="40" spans="2:17" ht="18.5">
-      <c r="B40" s="153"/>
+      <c r="B40" s="154"/>
       <c r="C40" s="35" t="s">
         <v>84</v>
       </c>
@@ -17412,12 +17412,12 @@
       </c>
     </row>
     <row r="41" spans="2:17">
-      <c r="B41" s="137" t="s">
+      <c r="B41" s="138" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="42" spans="2:17" ht="18.5">
-      <c r="B42" s="137"/>
+      <c r="B42" s="138"/>
       <c r="C42" s="101" t="s">
         <v>134</v>
       </c>
@@ -17433,7 +17433,7 @@
       </c>
     </row>
     <row r="43" spans="2:17" ht="18.5">
-      <c r="B43" s="137"/>
+      <c r="B43" s="138"/>
       <c r="C43" s="101" t="s">
         <v>139</v>
       </c>
@@ -17449,7 +17449,7 @@
       </c>
     </row>
     <row r="44" spans="2:17" ht="18.5">
-      <c r="B44" s="137"/>
+      <c r="B44" s="138"/>
       <c r="C44" s="101" t="s">
         <v>136</v>
       </c>
@@ -17465,7 +17465,7 @@
       </c>
     </row>
     <row r="45" spans="2:17" ht="18.5">
-      <c r="B45" s="137"/>
+      <c r="B45" s="138"/>
       <c r="C45" s="101" t="s">
         <v>135</v>
       </c>
@@ -17757,8 +17757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:L80"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="R68" sqref="R68"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -17819,7 +17819,7 @@
       </c>
       <c r="C8" s="65">
         <f>AVERAGE(C35:L35)</f>
-        <v>0.75395455593523353</v>
+        <v>0.88626859754841403</v>
       </c>
     </row>
     <row r="9" spans="2:12">
@@ -18511,7 +18511,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="24">
-        <f t="shared" ref="C35:K35" si="7">C28/C19</f>
+        <f t="shared" ref="C35:L35" si="7">C28/C19</f>
         <v>0.54005281690140849</v>
       </c>
       <c r="D35" s="24">
@@ -18546,7 +18546,10 @@
         <f t="shared" si="7"/>
         <v>0.93862560915318882</v>
       </c>
-      <c r="L35" s="24"/>
+      <c r="L35" s="24">
+        <f t="shared" si="7"/>
+        <v>2.0770949720670391</v>
+      </c>
     </row>
     <row r="38" spans="2:12" ht="20" thickBot="1">
       <c r="B38" s="3" t="s">
@@ -18795,43 +18798,43 @@
       </c>
       <c r="C48" s="21">
         <f>C45*C8</f>
-        <v>11084.790786631389</v>
+        <v>13030.098309306186</v>
       </c>
       <c r="D48" s="21">
         <f>D45*C8</f>
-        <v>11394.056449578406</v>
+        <v>13393.638052135828</v>
       </c>
       <c r="E48" s="21">
         <f>E45*C8</f>
-        <v>11389.498826998575</v>
+        <v>13388.280596914976</v>
       </c>
       <c r="F48" s="21">
         <f>F45*C8</f>
-        <v>11503.393815268561</v>
+        <v>13522.163402884124</v>
       </c>
       <c r="G48" s="21">
         <f>G45*C8</f>
-        <v>11618.427753421245</v>
+        <v>13657.385036912965</v>
       </c>
       <c r="H48" s="21">
         <f>H45*C8</f>
-        <v>11734.612030955459</v>
+        <v>13793.958887282097</v>
       </c>
       <c r="I48" s="21">
         <f>I45*C8</f>
-        <v>11851.958151265013</v>
+        <v>13931.898476154916</v>
       </c>
       <c r="J48" s="21">
         <f>J45*C8</f>
-        <v>11970.477732777663</v>
+        <v>14071.217460916467</v>
       </c>
       <c r="K48" s="21">
         <f>K45*C8</f>
-        <v>12090.18251010544</v>
+        <v>14211.92963552563</v>
       </c>
       <c r="L48" s="21">
         <f>L45*C8</f>
-        <v>12211.084335206495</v>
+        <v>14354.048931880889</v>
       </c>
     </row>
     <row r="49" spans="2:12">
@@ -18840,43 +18843,43 @@
       </c>
       <c r="C49" s="20">
         <f>(C48-L28)/L28</f>
-        <v>-6.2048783726565372E-3</v>
+        <v>0.16819959739162507</v>
       </c>
       <c r="D49" s="20">
         <f>(D48-C48)/C48</f>
-        <v>2.7900000000000078E-2</v>
+        <v>2.7899999999999949E-2</v>
       </c>
       <c r="E49" s="20">
         <f t="shared" ref="E49:L49" si="10">(E48-D48)/D48</f>
-        <v>-3.9999999999991751E-4</v>
+        <v>-3.9999999999982514E-4</v>
       </c>
       <c r="F49" s="20">
         <f t="shared" si="10"/>
-        <v>9.9999999999999638E-3</v>
+        <v>9.9999999999998493E-3</v>
       </c>
       <c r="G49" s="20">
         <f t="shared" si="10"/>
-        <v>9.9999999999999169E-3</v>
+        <v>1.0000000000000014E-2</v>
       </c>
       <c r="H49" s="20">
         <f t="shared" si="10"/>
-        <v>1.0000000000000118E-2</v>
+        <v>1.000000000000016E-2</v>
       </c>
       <c r="I49" s="20">
         <f t="shared" si="10"/>
-        <v>9.9999999999999464E-3</v>
+        <v>9.9999999999998944E-3</v>
       </c>
       <c r="J49" s="20">
         <f t="shared" si="10"/>
-        <v>9.9999999999999794E-3</v>
+        <v>1.0000000000000087E-2</v>
       </c>
       <c r="K49" s="20">
         <f t="shared" si="10"/>
-        <v>1.0000000000000054E-2</v>
+        <v>9.99999999999991E-3</v>
       </c>
       <c r="L49" s="20">
         <f t="shared" si="10"/>
-        <v>1.0000000000000031E-2</v>
+        <v>1.0000000000000153E-2</v>
       </c>
     </row>
     <row r="51" spans="2:12">
@@ -19076,43 +19079,43 @@
       </c>
       <c r="C59" s="21">
         <f t="shared" ref="C59:L59" si="12">C48/C57</f>
-        <v>10373.091888869758</v>
+        <v>12193.500958669398</v>
       </c>
       <c r="D59" s="21">
         <f t="shared" si="12"/>
-        <v>9977.9153571550614</v>
+        <v>11728.973557396001</v>
       </c>
       <c r="E59" s="21">
         <f t="shared" si="12"/>
-        <v>9333.548473532499</v>
+        <v>10971.524544376354</v>
       </c>
       <c r="F59" s="21">
         <f t="shared" si="12"/>
-        <v>8821.6309542582749</v>
+        <v>10369.768883778417</v>
       </c>
       <c r="G59" s="21">
         <f t="shared" si="12"/>
-        <v>8337.7905963426729</v>
+        <v>9801.0177407930569</v>
       </c>
       <c r="H59" s="21">
         <f t="shared" si="12"/>
-        <v>7880.4874505550488</v>
+        <v>9263.4609152773155</v>
       </c>
       <c r="I59" s="21">
         <f t="shared" si="12"/>
-        <v>7448.2660293239269</v>
+        <v>8755.3874912103674</v>
       </c>
       <c r="J59" s="21">
         <f t="shared" si="12"/>
-        <v>7039.7506742648775</v>
+        <v>8275.1803912531705</v>
       </c>
       <c r="K59" s="21">
         <f t="shared" si="12"/>
-        <v>6653.6411777857984</v>
+        <v>7821.3112299743907</v>
       </c>
       <c r="L59" s="21">
         <f t="shared" si="12"/>
-        <v>6288.7086448341797</v>
+        <v>7392.335449361688</v>
       </c>
     </row>
     <row r="60" spans="2:12">
@@ -19160,32 +19163,32 @@
       <c r="L62" s="21"/>
     </row>
     <row r="63" spans="2:12">
-      <c r="B63" s="157" t="s">
+      <c r="B63" s="158" t="s">
         <v>103</v>
       </c>
-      <c r="C63" s="157"/>
-      <c r="D63" s="157"/>
-      <c r="E63" s="157"/>
-      <c r="F63" s="157"/>
-      <c r="G63" s="157"/>
-      <c r="H63" s="157"/>
-      <c r="I63" s="157"/>
-      <c r="J63" s="157"/>
-      <c r="K63" s="157"/>
-      <c r="L63" s="157"/>
+      <c r="C63" s="158"/>
+      <c r="D63" s="158"/>
+      <c r="E63" s="158"/>
+      <c r="F63" s="158"/>
+      <c r="G63" s="158"/>
+      <c r="H63" s="158"/>
+      <c r="I63" s="158"/>
+      <c r="J63" s="158"/>
+      <c r="K63" s="158"/>
+      <c r="L63" s="158"/>
     </row>
     <row r="64" spans="2:12">
-      <c r="B64" s="157"/>
-      <c r="C64" s="157"/>
-      <c r="D64" s="157"/>
-      <c r="E64" s="157"/>
-      <c r="F64" s="157"/>
-      <c r="G64" s="157"/>
-      <c r="H64" s="157"/>
-      <c r="I64" s="157"/>
-      <c r="J64" s="157"/>
-      <c r="K64" s="157"/>
-      <c r="L64" s="157"/>
+      <c r="B64" s="158"/>
+      <c r="C64" s="158"/>
+      <c r="D64" s="158"/>
+      <c r="E64" s="158"/>
+      <c r="F64" s="158"/>
+      <c r="G64" s="158"/>
+      <c r="H64" s="158"/>
+      <c r="I64" s="158"/>
+      <c r="J64" s="158"/>
+      <c r="K64" s="158"/>
+      <c r="L64" s="158"/>
     </row>
     <row r="65" spans="2:12">
       <c r="B65" s="18" t="s">
@@ -19193,7 +19196,7 @@
       </c>
       <c r="C65" s="25">
         <f>L59*(1+C5)/(C4-C5)</f>
-        <v>147808.09929552308</v>
+        <v>173747.4438448688</v>
       </c>
     </row>
     <row r="66" spans="2:12" ht="15" thickBot="1">
@@ -19202,7 +19205,7 @@
       </c>
       <c r="C66" s="23">
         <f>C65/C61</f>
-        <v>71233.81439828701</v>
+        <v>83734.878034501948</v>
       </c>
     </row>
     <row r="67" spans="2:12" ht="15" thickTop="1"/>
@@ -19212,7 +19215,7 @@
       </c>
       <c r="C68" s="71">
         <f>(SUM(C59:L59)+C65)</f>
-        <v>229962.93054244519</v>
+        <v>270319.90500695899</v>
       </c>
     </row>
     <row r="69" spans="2:12" ht="15" thickTop="1">
@@ -19224,38 +19227,38 @@
       </c>
       <c r="C70" s="70">
         <f>C68/(C11/1000000)</f>
-        <v>54.667017807155744</v>
+        <v>64.260718133075443</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="30"/>
     </row>
     <row r="73" spans="2:12">
-      <c r="B73" s="157" t="s">
+      <c r="B73" s="158" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="157"/>
-      <c r="D73" s="157"/>
-      <c r="E73" s="157"/>
-      <c r="F73" s="157"/>
-      <c r="G73" s="157"/>
-      <c r="H73" s="157"/>
-      <c r="I73" s="157"/>
-      <c r="J73" s="157"/>
-      <c r="K73" s="157"/>
-      <c r="L73" s="157"/>
+      <c r="C73" s="158"/>
+      <c r="D73" s="158"/>
+      <c r="E73" s="158"/>
+      <c r="F73" s="158"/>
+      <c r="G73" s="158"/>
+      <c r="H73" s="158"/>
+      <c r="I73" s="158"/>
+      <c r="J73" s="158"/>
+      <c r="K73" s="158"/>
+      <c r="L73" s="158"/>
     </row>
     <row r="74" spans="2:12">
-      <c r="B74" s="157"/>
-      <c r="C74" s="157"/>
-      <c r="D74" s="157"/>
-      <c r="E74" s="157"/>
-      <c r="F74" s="157"/>
-      <c r="G74" s="157"/>
-      <c r="H74" s="157"/>
-      <c r="I74" s="157"/>
-      <c r="J74" s="157"/>
-      <c r="K74" s="157"/>
-      <c r="L74" s="157"/>
+      <c r="B74" s="158"/>
+      <c r="C74" s="158"/>
+      <c r="D74" s="158"/>
+      <c r="E74" s="158"/>
+      <c r="F74" s="158"/>
+      <c r="G74" s="158"/>
+      <c r="H74" s="158"/>
+      <c r="I74" s="158"/>
+      <c r="J74" s="158"/>
+      <c r="K74" s="158"/>
+      <c r="L74" s="158"/>
     </row>
     <row r="75" spans="2:12">
       <c r="B75" s="18" t="s">
@@ -19285,7 +19288,7 @@
       </c>
       <c r="C78" s="72">
         <f>SUM(C59:L59)+C76</f>
-        <v>208760.54809047969</v>
+        <v>223178.17800564773</v>
       </c>
     </row>
     <row r="79" spans="2:12" ht="15" thickTop="1"/>
@@ -19295,7 +19298,7 @@
       </c>
       <c r="C80" s="70">
         <f>C78/(C11/1000000)</f>
-        <v>49.626766248690807</v>
+        <v>53.054139649483318</v>
       </c>
     </row>
   </sheetData>
@@ -19416,10 +19419,10 @@
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1"/>
     <row r="4" spans="2:16" ht="20" thickBot="1">
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="161" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="161"/>
+      <c r="C4" s="162"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1">
       <c r="B5" s="81" t="s">
@@ -19480,10 +19483,10 @@
       <c r="L6" s="88">
         <v>10</v>
       </c>
-      <c r="M6" s="162" t="s">
+      <c r="M6" s="163" t="s">
         <v>125</v>
       </c>
-      <c r="N6" s="163"/>
+      <c r="N6" s="164"/>
       <c r="O6" s="89" t="s">
         <v>126</v>
       </c>
@@ -19536,11 +19539,11 @@
         <f>K7*(1+P7)</f>
         <v>1.3824913077320653</v>
       </c>
-      <c r="M7" s="158">
+      <c r="M7" s="159">
         <f>L7*(1+P7)/(P8-P7)</f>
         <v>32.49370006293983</v>
       </c>
-      <c r="N7" s="159"/>
+      <c r="N7" s="160"/>
       <c r="O7" s="89" t="s">
         <v>128</v>
       </c>
@@ -19592,11 +19595,11 @@
         <f>L7/(1+P8)^10</f>
         <v>0.71198304750679042</v>
       </c>
-      <c r="M8" s="158">
+      <c r="M8" s="159">
         <f>M7/POWER((1+P8),10)</f>
         <v>16.734256097085837</v>
       </c>
-      <c r="N8" s="159"/>
+      <c r="N8" s="160"/>
       <c r="O8" s="92" t="s">
         <v>130</v>
       </c>
@@ -19637,10 +19640,10 @@
       <c r="O12" s="100"/>
     </row>
     <row r="13" spans="2:16" ht="20" thickBot="1">
-      <c r="B13" s="160" t="s">
+      <c r="B13" s="161" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="161"/>
+      <c r="C13" s="162"/>
     </row>
     <row r="14" spans="2:16" ht="15" thickBot="1">
       <c r="B14" s="81" t="s">
@@ -19701,10 +19704,10 @@
       <c r="L15" s="88">
         <v>10</v>
       </c>
-      <c r="M15" s="162" t="s">
+      <c r="M15" s="163" t="s">
         <v>125</v>
       </c>
-      <c r="N15" s="163"/>
+      <c r="N15" s="164"/>
       <c r="O15" s="89" t="s">
         <v>126</v>
       </c>
@@ -19757,11 +19760,11 @@
         <f>K16*(1+P16)</f>
         <v>1.4514296896916519</v>
       </c>
-      <c r="M16" s="158">
+      <c r="M16" s="159">
         <f>L16*(1+P16)/(P17-P16)</f>
         <v>38.719725758083044</v>
       </c>
-      <c r="N16" s="159"/>
+      <c r="N16" s="160"/>
       <c r="O16" s="89" t="s">
         <v>128</v>
       </c>
@@ -19813,11 +19816,11 @@
         <f>L16/(1+P17)^10</f>
         <v>0.74748631541398081</v>
       </c>
-      <c r="M17" s="158">
+      <c r="M17" s="159">
         <f>M16/POWER((1+P17),10)</f>
         <v>19.940659438279759</v>
       </c>
-      <c r="N17" s="159"/>
+      <c r="N17" s="160"/>
       <c r="O17" s="92" t="s">
         <v>130</v>
       </c>
@@ -19852,10 +19855,10 @@
     </row>
     <row r="21" spans="2:16" ht="15" thickBot="1"/>
     <row r="22" spans="2:16" ht="20" thickBot="1">
-      <c r="B22" s="160" t="s">
+      <c r="B22" s="161" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="161"/>
+      <c r="C22" s="162"/>
     </row>
     <row r="23" spans="2:16" ht="15" thickBot="1">
       <c r="B23" s="81" t="s">
@@ -19916,10 +19919,10 @@
       <c r="L24" s="88">
         <v>10</v>
       </c>
-      <c r="M24" s="162" t="s">
+      <c r="M24" s="163" t="s">
         <v>125</v>
       </c>
-      <c r="N24" s="163"/>
+      <c r="N24" s="164"/>
       <c r="O24" s="89" t="s">
         <v>126</v>
       </c>
@@ -19972,11 +19975,11 @@
         <f>K25*(1+P25)</f>
         <v>1.5234466614708106</v>
       </c>
-      <c r="M25" s="158">
+      <c r="M25" s="159">
         <f>L25*(1+P25)/(P26-P25)</f>
         <v>46.91349258789446</v>
       </c>
-      <c r="N25" s="159"/>
+      <c r="N25" s="160"/>
       <c r="O25" s="89" t="s">
         <v>128</v>
       </c>
@@ -20028,11 +20031,11 @@
         <f>L25/(1+P26)^10</f>
         <v>0.78457505713175035</v>
       </c>
-      <c r="M26" s="158">
+      <c r="M26" s="159">
         <f>M25/POWER((1+P26),10)</f>
         <v>24.160449498022988</v>
       </c>
-      <c r="N26" s="159"/>
+      <c r="N26" s="160"/>
       <c r="O26" s="92" t="s">
         <v>130</v>
       </c>

</xml_diff>

<commit_message>
Updates on excel and ddm and graham for JNJ and UNP.
</commit_message>
<xml_diff>
--- a/src/main/resources/companies/template.xlsx
+++ b/src/main/resources/companies/template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C22D9A-4730-413B-B632-FE39C21E0A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D99114E-BCE0-43CD-A31C-362704162A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valuation Metrics" sheetId="5" r:id="rId1"/>
@@ -16483,7 +16483,7 @@
   <dimension ref="B2:V45"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -17132,7 +17132,7 @@
         <v>160</v>
       </c>
       <c r="F24" s="57">
-        <f>AVERAGE(L24:P24)</f>
+        <f>AVERAGEIF(L24:P24,"&lt;100")</f>
         <v>18.525999927520751</v>
       </c>
       <c r="G24" s="44">
@@ -17213,7 +17213,7 @@
         <v>160</v>
       </c>
       <c r="F26" s="57">
-        <f>AVERAGE(L26:P26)</f>
+        <f>AVERAGEIF(L26:P26, "&lt;100")</f>
         <v>7.7179999351501465</v>
       </c>
       <c r="G26" s="44">
@@ -17809,8 +17809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:L80"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -17870,8 +17870,8 @@
         <v>114</v>
       </c>
       <c r="C8" s="65">
-        <f>AVERAGE(C35:L35)</f>
-        <v>0.88626859754841403</v>
+        <f>AVERAGEIF(C35:L35,"&lt;2")</f>
+        <v>0.75395455593523353</v>
       </c>
     </row>
     <row r="9" spans="2:12">
@@ -18850,43 +18850,43 @@
       </c>
       <c r="C48" s="21">
         <f>C45*C8</f>
-        <v>13030.098309306186</v>
+        <v>11084.790786631389</v>
       </c>
       <c r="D48" s="21">
         <f>D45*C8</f>
-        <v>13393.638052135828</v>
+        <v>11394.056449578406</v>
       </c>
       <c r="E48" s="21">
         <f>E45*C8</f>
-        <v>13388.280596914976</v>
+        <v>11389.498826998575</v>
       </c>
       <c r="F48" s="21">
         <f>F45*C8</f>
-        <v>13522.163402884124</v>
+        <v>11503.393815268561</v>
       </c>
       <c r="G48" s="21">
         <f>G45*C8</f>
-        <v>13657.385036912965</v>
+        <v>11618.427753421245</v>
       </c>
       <c r="H48" s="21">
         <f>H45*C8</f>
-        <v>13793.958887282097</v>
+        <v>11734.612030955459</v>
       </c>
       <c r="I48" s="21">
         <f>I45*C8</f>
-        <v>13931.898476154916</v>
+        <v>11851.958151265013</v>
       </c>
       <c r="J48" s="21">
         <f>J45*C8</f>
-        <v>14071.217460916467</v>
+        <v>11970.477732777663</v>
       </c>
       <c r="K48" s="21">
         <f>K45*C8</f>
-        <v>14211.92963552563</v>
+        <v>12090.18251010544</v>
       </c>
       <c r="L48" s="21">
         <f>L45*C8</f>
-        <v>14354.048931880889</v>
+        <v>12211.084335206495</v>
       </c>
     </row>
     <row r="49" spans="2:12">
@@ -18895,43 +18895,43 @@
       </c>
       <c r="C49" s="20">
         <f>(C48-L28)/L28</f>
-        <v>0.16819959739162507</v>
+        <v>-6.2048783726565372E-3</v>
       </c>
       <c r="D49" s="20">
         <f>(D48-C48)/C48</f>
-        <v>2.7899999999999949E-2</v>
+        <v>2.7900000000000078E-2</v>
       </c>
       <c r="E49" s="20">
         <f t="shared" ref="E49:L49" si="10">(E48-D48)/D48</f>
-        <v>-3.9999999999982514E-4</v>
+        <v>-3.9999999999991751E-4</v>
       </c>
       <c r="F49" s="20">
         <f t="shared" si="10"/>
-        <v>9.9999999999998493E-3</v>
+        <v>9.9999999999999638E-3</v>
       </c>
       <c r="G49" s="20">
         <f t="shared" si="10"/>
-        <v>1.0000000000000014E-2</v>
+        <v>9.9999999999999169E-3</v>
       </c>
       <c r="H49" s="20">
         <f t="shared" si="10"/>
-        <v>1.000000000000016E-2</v>
+        <v>1.0000000000000118E-2</v>
       </c>
       <c r="I49" s="20">
         <f t="shared" si="10"/>
-        <v>9.9999999999998944E-3</v>
+        <v>9.9999999999999464E-3</v>
       </c>
       <c r="J49" s="20">
         <f t="shared" si="10"/>
-        <v>1.0000000000000087E-2</v>
+        <v>9.9999999999999794E-3</v>
       </c>
       <c r="K49" s="20">
         <f t="shared" si="10"/>
-        <v>9.99999999999991E-3</v>
+        <v>1.0000000000000054E-2</v>
       </c>
       <c r="L49" s="20">
         <f t="shared" si="10"/>
-        <v>1.0000000000000153E-2</v>
+        <v>1.0000000000000031E-2</v>
       </c>
     </row>
     <row r="51" spans="2:12">
@@ -19131,43 +19131,43 @@
       </c>
       <c r="C59" s="21">
         <f t="shared" ref="C59:L59" si="12">C48/C57</f>
-        <v>12193.500958669398</v>
+        <v>10373.091888869758</v>
       </c>
       <c r="D59" s="21">
         <f t="shared" si="12"/>
-        <v>11728.973557396001</v>
+        <v>9977.9153571550614</v>
       </c>
       <c r="E59" s="21">
         <f t="shared" si="12"/>
-        <v>10971.524544376354</v>
+        <v>9333.548473532499</v>
       </c>
       <c r="F59" s="21">
         <f t="shared" si="12"/>
-        <v>10369.768883778417</v>
+        <v>8821.6309542582749</v>
       </c>
       <c r="G59" s="21">
         <f t="shared" si="12"/>
-        <v>9801.0177407930569</v>
+        <v>8337.7905963426729</v>
       </c>
       <c r="H59" s="21">
         <f t="shared" si="12"/>
-        <v>9263.4609152773137</v>
+        <v>7880.4874505550479</v>
       </c>
       <c r="I59" s="21">
         <f t="shared" si="12"/>
-        <v>8755.3874912103656</v>
+        <v>7448.266029323926</v>
       </c>
       <c r="J59" s="21">
         <f t="shared" si="12"/>
-        <v>8275.1803912531686</v>
+        <v>7039.7506742648766</v>
       </c>
       <c r="K59" s="21">
         <f t="shared" si="12"/>
-        <v>7821.3112299743898</v>
+        <v>6653.6411777857975</v>
       </c>
       <c r="L59" s="21">
         <f t="shared" si="12"/>
-        <v>7392.3354493616862</v>
+        <v>6288.7086448341788</v>
       </c>
     </row>
     <row r="60" spans="2:12">
@@ -19248,7 +19248,7 @@
       </c>
       <c r="C65" s="25">
         <f>L59*(1+C5)/(C4-C5)</f>
-        <v>173747.44384486874</v>
+        <v>147808.09929552305</v>
       </c>
     </row>
     <row r="66" spans="2:12" ht="15" thickBot="1">
@@ -19257,7 +19257,7 @@
       </c>
       <c r="C66" s="23">
         <f>C65/C61</f>
-        <v>83734.878034501904</v>
+        <v>71233.814398286981</v>
       </c>
     </row>
     <row r="67" spans="2:12" ht="15" thickTop="1"/>
@@ -19267,7 +19267,7 @@
       </c>
       <c r="C68" s="71">
         <f>(SUM(C59:L59)+C65)</f>
-        <v>270319.90500695887</v>
+        <v>229962.93054244516</v>
       </c>
     </row>
     <row r="69" spans="2:12" ht="15" thickTop="1">
@@ -19279,7 +19279,7 @@
       </c>
       <c r="C70" s="70">
         <f>C68/(C11/1000000)</f>
-        <v>64.260718133075414</v>
+        <v>54.667017807155737</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="30"/>
@@ -19340,7 +19340,7 @@
       </c>
       <c r="C78" s="72">
         <f>SUM(C59:L59)+C76</f>
-        <v>223178.17800564767</v>
+        <v>208760.54809047963</v>
       </c>
     </row>
     <row r="79" spans="2:12" ht="15" thickTop="1"/>
@@ -19350,7 +19350,7 @@
       </c>
       <c r="C80" s="70">
         <f>C78/(C11/1000000)</f>
-        <v>53.054139649483304</v>
+        <v>49.626766248690792</v>
       </c>
     </row>
   </sheetData>
@@ -19368,7 +19368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B13:E21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated with EBIDTA 3y forecast.
</commit_message>
<xml_diff>
--- a/src/main/resources/companies/template.xlsx
+++ b/src/main/resources/companies/template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D2C41D-A74C-45FB-8ED9-E98810C63079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A449CDF3-4847-49B3-B1C1-32D83E004718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valuation Metrics" sheetId="5" r:id="rId1"/>
@@ -18684,7 +18684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:V47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="75" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="75" workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
@@ -20113,8 +20113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:L74"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="82" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="82" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -21044,45 +21044,42 @@
       <c r="B45" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="21">
-        <f>L25*(1+C46)</f>
-        <v>1911.679998755455</v>
-      </c>
-      <c r="D45" s="21">
-        <f>C45*(1+D46)</f>
-        <v>1969.0303974362373</v>
-      </c>
-      <c r="E45" s="21">
-        <f t="shared" ref="E45:L45" si="8">D45*(1+E46)</f>
-        <v>2028.1013080389866</v>
+      <c r="C45" s="60">
+        <v>2801</v>
+      </c>
+      <c r="D45" s="60">
+        <v>3144</v>
+      </c>
+      <c r="E45" s="60">
+        <v>3405</v>
       </c>
       <c r="F45" s="21">
-        <f t="shared" si="8"/>
-        <v>2088.9443459202084</v>
+        <f t="shared" ref="E45:L45" si="8">E45*(1+F46)</f>
+        <v>3507.1499977167696</v>
       </c>
       <c r="G45" s="21">
         <f t="shared" si="8"/>
-        <v>2151.6126748970682</v>
+        <v>3612.3644952965451</v>
       </c>
       <c r="H45" s="21">
         <f t="shared" si="8"/>
-        <v>2216.1610537012116</v>
+        <v>3720.7354277331624</v>
       </c>
       <c r="I45" s="21">
         <f t="shared" si="8"/>
-        <v>2282.645883826196</v>
+        <v>3832.3574880702099</v>
       </c>
       <c r="J45" s="21">
         <f t="shared" si="8"/>
-        <v>2351.1252588103484</v>
+        <v>3947.3282101425202</v>
       </c>
       <c r="K45" s="21">
         <f t="shared" si="8"/>
-        <v>2421.6590149981066</v>
+        <v>4065.7480537999058</v>
       </c>
       <c r="L45" s="21">
         <f t="shared" si="8"/>
-        <v>2494.3087838242009</v>
+        <v>4187.7204926876066</v>
       </c>
     </row>
     <row r="46" spans="2:12">
@@ -21424,7 +21421,7 @@
       </c>
       <c r="C69" s="25">
         <f>L45*C9</f>
-        <v>29358.015527414791</v>
+        <v>49289.472115919438</v>
       </c>
     </row>
     <row r="70" spans="2:12" ht="15" thickBot="1">
@@ -21433,7 +21430,7 @@
       </c>
       <c r="C70" s="23">
         <f>C69/C55</f>
-        <v>14383.365015735828</v>
+        <v>24148.378428854616</v>
       </c>
     </row>
     <row r="71" spans="2:12" ht="15" thickTop="1">
@@ -21446,7 +21443,7 @@
       </c>
       <c r="C72" s="72">
         <f>SUM(C53:L53)+C70</f>
-        <v>26780.54195806678</v>
+        <v>36545.555371185568</v>
       </c>
     </row>
     <row r="73" spans="2:12" ht="15" thickTop="1"/>
@@ -21456,7 +21453,7 @@
       </c>
       <c r="C74" s="70">
         <f>C72/(C11/1000000)</f>
-        <v>246.88414142464259</v>
+        <v>336.90573084104966</v>
       </c>
     </row>
   </sheetData>
@@ -21552,7 +21549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>

</xml_diff>